<commit_message>
updating dual fuel and r32 heat pump models
</commit_message>
<xml_diff>
--- a/Data Scraping/output_h.xlsx
+++ b/Data Scraping/output_h.xlsx
@@ -11,6 +11,7 @@
     <sheet name="Sheet_name3" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="Sheet_name4" sheetId="3" state="visible" r:id="rId3"/>
     <sheet name="Sheet_name5" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Sheet_name6" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -428,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q10"/>
+  <dimension ref="A1:Q11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -574,51 +575,51 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>29.7</v>
+        <v>30.5</v>
       </c>
       <c r="D4" t="n">
-        <v>28.1</v>
+        <v>28.9</v>
       </c>
       <c r="E4" t="n">
-        <v>26.4</v>
+        <v>27.2</v>
       </c>
       <c r="F4" t="n">
-        <v>24.7</v>
+        <v>25.4</v>
       </c>
       <c r="G4" t="n">
-        <v>23.6</v>
+        <v>24.3</v>
       </c>
       <c r="H4" t="n">
-        <v>22.9</v>
+        <v>23.5</v>
       </c>
       <c r="I4" t="n">
-        <v>21.2</v>
+        <v>21.8</v>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>21.3 18.9 17.5 16.4</t>
+          <t>20.1 17.1 15.7 14.5</t>
         </is>
       </c>
       <c r="K4" t="n">
-        <v>15.2</v>
+        <v>13.7</v>
       </c>
       <c r="L4" t="n">
-        <v>14</v>
+        <v>13.2</v>
       </c>
       <c r="M4" t="n">
-        <v>12.7</v>
+        <v>11.8</v>
       </c>
       <c r="N4" t="n">
-        <v>11.4</v>
+        <v>10.5</v>
       </c>
       <c r="O4" t="n">
-        <v>10.3</v>
+        <v>9.1</v>
       </c>
       <c r="P4" t="n">
-        <v>8.9</v>
+        <v>7.8</v>
       </c>
       <c r="Q4" t="n">
-        <v>7.1</v>
+        <v>6.4</v>
       </c>
     </row>
     <row r="5">
@@ -631,51 +632,51 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>38</v>
+        <v>33.2</v>
       </c>
       <c r="D5" t="n">
-        <v>36</v>
+        <v>31.5</v>
       </c>
       <c r="E5" t="n">
-        <v>34</v>
+        <v>29.6</v>
       </c>
       <c r="F5" t="n">
-        <v>32</v>
+        <v>27.7</v>
       </c>
       <c r="G5" t="n">
-        <v>30</v>
+        <v>26.4</v>
       </c>
       <c r="H5" t="n">
-        <v>29</v>
+        <v>25.6</v>
       </c>
       <c r="I5" t="n">
-        <v>27</v>
+        <v>23.8</v>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>27 24 22 21</t>
+          <t>21.9 18.6 17.1 15.8</t>
         </is>
       </c>
       <c r="K5" t="n">
-        <v>20</v>
+        <v>14.9</v>
       </c>
       <c r="L5" t="n">
-        <v>18</v>
+        <v>14.4</v>
       </c>
       <c r="M5" t="n">
-        <v>16</v>
+        <v>12.9</v>
       </c>
       <c r="N5" t="n">
-        <v>15</v>
+        <v>11.4</v>
       </c>
       <c r="O5" t="n">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="P5" t="n">
-        <v>11</v>
+        <v>8.5</v>
       </c>
       <c r="Q5" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6">
@@ -688,51 +689,51 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>2.03</v>
+        <v>2.07</v>
       </c>
       <c r="D6" t="n">
-        <v>1.96</v>
+        <v>2.02</v>
       </c>
       <c r="E6" t="n">
-        <v>1.97</v>
+        <v>1.98</v>
       </c>
       <c r="F6" t="n">
-        <v>1.92</v>
+        <v>1.94</v>
       </c>
       <c r="G6" t="n">
-        <v>1.87</v>
+        <v>1.91</v>
       </c>
       <c r="H6" t="n">
+        <v>1.9</v>
+      </c>
+      <c r="I6" t="n">
         <v>1.86</v>
       </c>
-      <c r="I6" t="n">
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>1.81 2.04 1.99 1.94</t>
+        </is>
+      </c>
+      <c r="K6" t="n">
+        <v>1.91</v>
+      </c>
+      <c r="L6" t="n">
+        <v>1.89</v>
+      </c>
+      <c r="M6" t="n">
+        <v>1.84</v>
+      </c>
+      <c r="N6" t="n">
         <v>1.79</v>
       </c>
-      <c r="J6" t="inlineStr">
-        <is>
-          <t>2.01 1.91 1.86 1.85</t>
-        </is>
-      </c>
-      <c r="K6" t="n">
-        <v>1.82</v>
-      </c>
-      <c r="L6" t="n">
-        <v>1.74</v>
-      </c>
-      <c r="M6" t="n">
+      <c r="O6" t="n">
+        <v>1.75</v>
+      </c>
+      <c r="P6" t="n">
+        <v>1.69</v>
+      </c>
+      <c r="Q6" t="n">
         <v>1.65</v>
-      </c>
-      <c r="N6" t="n">
-        <v>1.6</v>
-      </c>
-      <c r="O6" t="n">
-        <v>1.56</v>
-      </c>
-      <c r="P6" t="n">
-        <v>1.51</v>
-      </c>
-      <c r="Q6" t="n">
-        <v>1.39</v>
       </c>
     </row>
     <row r="7">
@@ -745,51 +746,51 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>8.5</v>
+        <v>10.2</v>
       </c>
       <c r="D7" t="n">
+        <v>9.5</v>
+      </c>
+      <c r="E7" t="n">
+        <v>8.9</v>
+      </c>
+      <c r="F7" t="n">
+        <v>8.4</v>
+      </c>
+      <c r="G7" t="n">
         <v>8.1</v>
       </c>
-      <c r="E7" t="n">
-        <v>8.199999999999999</v>
-      </c>
-      <c r="F7" t="n">
-        <v>8</v>
-      </c>
-      <c r="G7" t="n">
-        <v>7.7</v>
-      </c>
       <c r="H7" t="n">
-        <v>7.7</v>
+        <v>7.9</v>
       </c>
       <c r="I7" t="n">
-        <v>7.4</v>
+        <v>7.5</v>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>8.4 7.9 7.7 7.7</t>
+          <t>7.1 6.9 6.6 6.3</t>
         </is>
       </c>
       <c r="K7" t="n">
-        <v>7.5</v>
+        <v>6.1</v>
       </c>
       <c r="L7" t="n">
-        <v>7.2</v>
+        <v>6.1</v>
       </c>
       <c r="M7" t="n">
-        <v>6.8</v>
+        <v>5.8</v>
       </c>
       <c r="N7" t="n">
-        <v>6.6</v>
+        <v>5.4</v>
       </c>
       <c r="O7" t="n">
-        <v>6.4</v>
+        <v>5.1</v>
       </c>
       <c r="P7" t="n">
-        <v>6.2</v>
+        <v>4.8</v>
       </c>
       <c r="Q7" t="n">
-        <v>5.7</v>
+        <v>4.3</v>
       </c>
     </row>
     <row r="8">
@@ -802,51 +803,51 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>4.28</v>
+        <v>4.32</v>
       </c>
       <c r="D8" t="n">
-        <v>4.2</v>
+        <v>4.18</v>
       </c>
       <c r="E8" t="n">
-        <v>3.94</v>
+        <v>4.02</v>
       </c>
       <c r="F8" t="n">
-        <v>3.78</v>
+        <v>3.84</v>
       </c>
       <c r="G8" t="n">
-        <v>3.7</v>
+        <v>3.71</v>
       </c>
       <c r="H8" t="n">
-        <v>3.61</v>
+        <v>3.63</v>
       </c>
       <c r="I8" t="n">
-        <v>3.48</v>
+        <v>3.45</v>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>3.10 2.90 2.75 2.60</t>
+          <t>3.25 2.44 2.31 2.18</t>
         </is>
       </c>
       <c r="K8" t="n">
-        <v>2.45</v>
+        <v>2.09</v>
       </c>
       <c r="L8" t="n">
-        <v>2.36</v>
+        <v>2.04</v>
       </c>
       <c r="M8" t="n">
-        <v>2.25</v>
+        <v>1.88</v>
       </c>
       <c r="N8" t="n">
-        <v>2.09</v>
+        <v>1.71</v>
       </c>
       <c r="O8" t="n">
-        <v>1.93</v>
+        <v>1.53</v>
       </c>
       <c r="P8" t="n">
-        <v>1.72</v>
+        <v>1.35</v>
       </c>
       <c r="Q8" t="n">
-        <v>1.5</v>
+        <v>1.14</v>
       </c>
     </row>
     <row r="9">
@@ -855,55 +856,55 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>HI PR</t>
+          <t>EER</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>486</v>
+        <v>14.8</v>
       </c>
       <c r="D9" t="n">
-        <v>467</v>
+        <v>14.3</v>
       </c>
       <c r="E9" t="n">
-        <v>452</v>
+        <v>13.7</v>
       </c>
       <c r="F9" t="n">
-        <v>439</v>
+        <v>13.1</v>
       </c>
       <c r="G9" t="n">
-        <v>427</v>
+        <v>12.7</v>
       </c>
       <c r="H9" t="n">
-        <v>421</v>
+        <v>12.4</v>
       </c>
       <c r="I9" t="n">
-        <v>410</v>
+        <v>11.8</v>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>323 312 304 296</t>
+          <t>11.1 8.3 7.9 7.5</t>
         </is>
       </c>
       <c r="K9" t="n">
-        <v>292</v>
+        <v>7.2</v>
       </c>
       <c r="L9" t="n">
-        <v>288</v>
+        <v>7</v>
       </c>
       <c r="M9" t="n">
-        <v>281</v>
+        <v>6.4</v>
       </c>
       <c r="N9" t="n">
-        <v>274</v>
+        <v>5.8</v>
       </c>
       <c r="O9" t="n">
-        <v>268</v>
+        <v>5.2</v>
       </c>
       <c r="P9" t="n">
-        <v>262</v>
+        <v>4.6</v>
       </c>
       <c r="Q9" t="n">
-        <v>256</v>
+        <v>3.9</v>
       </c>
     </row>
     <row r="10">
@@ -912,55 +913,112 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
+          <t>HI PR</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>411</v>
+      </c>
+      <c r="D10" t="n">
+        <v>394</v>
+      </c>
+      <c r="E10" t="n">
+        <v>379</v>
+      </c>
+      <c r="F10" t="n">
+        <v>362</v>
+      </c>
+      <c r="G10" t="n">
+        <v>354</v>
+      </c>
+      <c r="H10" t="n">
+        <v>347</v>
+      </c>
+      <c r="I10" t="n">
+        <v>334</v>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>320 307 293 281</t>
+        </is>
+      </c>
+      <c r="K10" t="n">
+        <v>275</v>
+      </c>
+      <c r="L10" t="n">
+        <v>270</v>
+      </c>
+      <c r="M10" t="n">
+        <v>259</v>
+      </c>
+      <c r="N10" t="n">
+        <v>249</v>
+      </c>
+      <c r="O10" t="n">
+        <v>239</v>
+      </c>
+      <c r="P10" t="n">
+        <v>231</v>
+      </c>
+      <c r="Q10" t="n">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
           <t>LO PR</t>
         </is>
       </c>
-      <c r="C10" t="n">
-        <v>150</v>
-      </c>
-      <c r="D10" t="n">
-        <v>138</v>
-      </c>
-      <c r="E10" t="n">
-        <v>127</v>
-      </c>
-      <c r="F10" t="n">
-        <v>118</v>
-      </c>
-      <c r="G10" t="n">
-        <v>109</v>
-      </c>
-      <c r="H10" t="n">
-        <v>108</v>
-      </c>
-      <c r="I10" t="n">
-        <v>99</v>
-      </c>
-      <c r="J10" t="inlineStr">
-        <is>
-          <t>91 83 75 68</t>
-        </is>
-      </c>
-      <c r="K10" t="n">
-        <v>61</v>
-      </c>
-      <c r="L10" t="n">
-        <v>61</v>
-      </c>
-      <c r="M10" t="n">
-        <v>54</v>
-      </c>
-      <c r="N10" t="n">
-        <v>48</v>
-      </c>
-      <c r="O10" t="n">
-        <v>42</v>
-      </c>
-      <c r="P10" t="n">
-        <v>36</v>
-      </c>
-      <c r="Q10" t="n">
-        <v>31</v>
+      <c r="C11" t="n">
+        <v>141</v>
+      </c>
+      <c r="D11" t="n">
+        <v>130</v>
+      </c>
+      <c r="E11" t="n">
+        <v>122</v>
+      </c>
+      <c r="F11" t="n">
+        <v>112</v>
+      </c>
+      <c r="G11" t="n">
+        <v>106</v>
+      </c>
+      <c r="H11" t="n">
+        <v>102</v>
+      </c>
+      <c r="I11" t="n">
+        <v>94</v>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>83 75 67 59</t>
+        </is>
+      </c>
+      <c r="K11" t="n">
+        <v>55</v>
+      </c>
+      <c r="L11" t="n">
+        <v>53</v>
+      </c>
+      <c r="M11" t="n">
+        <v>45</v>
+      </c>
+      <c r="N11" t="n">
+        <v>39</v>
+      </c>
+      <c r="O11" t="n">
+        <v>33</v>
+      </c>
+      <c r="P11" t="n">
+        <v>28</v>
+      </c>
+      <c r="Q11" t="n">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -974,7 +1032,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q10"/>
+  <dimension ref="A1:Q11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1120,51 +1178,51 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>44</v>
+        <v>36.3</v>
       </c>
       <c r="D4" t="n">
-        <v>41.7</v>
+        <v>34.4</v>
       </c>
       <c r="E4" t="n">
-        <v>39.2</v>
+        <v>32.3</v>
       </c>
       <c r="F4" t="n">
-        <v>36.6</v>
+        <v>30.2</v>
       </c>
       <c r="G4" t="n">
-        <v>35</v>
+        <v>28.9</v>
       </c>
       <c r="H4" t="n">
-        <v>33.9</v>
+        <v>28</v>
       </c>
       <c r="I4" t="n">
-        <v>31.5</v>
+        <v>26</v>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>38.8 35.9 33.1 30.5</t>
+          <t>24.0 20.6 19.1 17.5</t>
         </is>
       </c>
       <c r="K4" t="n">
-        <v>28.8</v>
+        <v>16.6</v>
       </c>
       <c r="L4" t="n">
-        <v>27.7</v>
+        <v>16</v>
       </c>
       <c r="M4" t="n">
-        <v>24.9</v>
+        <v>14.3</v>
       </c>
       <c r="N4" t="n">
-        <v>22.1</v>
+        <v>12.7</v>
       </c>
       <c r="O4" t="n">
-        <v>19.2</v>
+        <v>11.1</v>
       </c>
       <c r="P4" t="n">
-        <v>16.4</v>
+        <v>9.4</v>
       </c>
       <c r="Q4" t="n">
-        <v>13.4</v>
+        <v>7.7</v>
       </c>
     </row>
     <row r="5">
@@ -1177,51 +1235,51 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>35</v>
+        <v>32.3</v>
       </c>
       <c r="D5" t="n">
-        <v>33</v>
+        <v>30.6</v>
       </c>
       <c r="E5" t="n">
-        <v>31</v>
+        <v>28.8</v>
       </c>
       <c r="F5" t="n">
-        <v>29</v>
+        <v>26.9</v>
       </c>
       <c r="G5" t="n">
-        <v>28</v>
+        <v>25.7</v>
       </c>
       <c r="H5" t="n">
-        <v>27</v>
+        <v>24.9</v>
       </c>
       <c r="I5" t="n">
-        <v>25</v>
+        <v>23.1</v>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>31 29 26 24</t>
+          <t>21.3 18.4 17.0 15.6</t>
         </is>
       </c>
       <c r="K5" t="n">
-        <v>23</v>
+        <v>14.7</v>
       </c>
       <c r="L5" t="n">
-        <v>22</v>
+        <v>14.2</v>
       </c>
       <c r="M5" t="n">
-        <v>20</v>
+        <v>12.7</v>
       </c>
       <c r="N5" t="n">
-        <v>18</v>
+        <v>11.3</v>
       </c>
       <c r="O5" t="n">
-        <v>15</v>
+        <v>9.9</v>
       </c>
       <c r="P5" t="n">
-        <v>13</v>
+        <v>8.4</v>
       </c>
       <c r="Q5" t="n">
-        <v>11</v>
+        <v>6.9</v>
       </c>
     </row>
     <row r="6">
@@ -1234,51 +1292,51 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>2.66</v>
+        <v>2.54</v>
       </c>
       <c r="D6" t="n">
-        <v>2.61</v>
+        <v>2.49</v>
       </c>
       <c r="E6" t="n">
-        <v>2.56</v>
+        <v>2.44</v>
       </c>
       <c r="F6" t="n">
-        <v>2.51</v>
+        <v>2.39</v>
       </c>
       <c r="G6" t="n">
-        <v>2.48</v>
+        <v>2.36</v>
       </c>
       <c r="H6" t="n">
-        <v>2.46</v>
+        <v>2.34</v>
       </c>
       <c r="I6" t="n">
-        <v>2.41</v>
+        <v>2.29</v>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>4.06 3.97 3.87 3.77</t>
+          <t>2.24 2.12 2.07 2.02</t>
         </is>
       </c>
       <c r="K6" t="n">
-        <v>3.72</v>
+        <v>1.99</v>
       </c>
       <c r="L6" t="n">
-        <v>3.68</v>
+        <v>1.97</v>
       </c>
       <c r="M6" t="n">
-        <v>3.58</v>
+        <v>1.92</v>
       </c>
       <c r="N6" t="n">
-        <v>3.48</v>
+        <v>1.88</v>
       </c>
       <c r="O6" t="n">
-        <v>3.39</v>
+        <v>1.83</v>
       </c>
       <c r="P6" t="n">
-        <v>3.29</v>
+        <v>1.78</v>
       </c>
       <c r="Q6" t="n">
-        <v>3.19</v>
+        <v>1.73</v>
       </c>
     </row>
     <row r="7">
@@ -1291,51 +1349,51 @@
         </is>
       </c>
       <c r="C7" t="n">
+        <v>13</v>
+      </c>
+      <c r="D7" t="n">
+        <v>12.1</v>
+      </c>
+      <c r="E7" t="n">
+        <v>11.4</v>
+      </c>
+      <c r="F7" t="n">
         <v>10.8</v>
       </c>
-      <c r="D7" t="n">
+      <c r="G7" t="n">
         <v>10.5</v>
       </c>
-      <c r="E7" t="n">
+      <c r="H7" t="n">
         <v>10.3</v>
       </c>
-      <c r="F7" t="n">
-        <v>10.1</v>
-      </c>
-      <c r="G7" t="n">
-        <v>10</v>
-      </c>
-      <c r="H7" t="n">
-        <v>9.9</v>
-      </c>
       <c r="I7" t="n">
-        <v>9.699999999999999</v>
+        <v>9.800000000000001</v>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>16.9 16.4 16.0 15.6</t>
+          <t>9.3 9.0 8.7 8.3</t>
         </is>
       </c>
       <c r="K7" t="n">
-        <v>15.3</v>
+        <v>8.1</v>
       </c>
       <c r="L7" t="n">
-        <v>15.2</v>
+        <v>8.1</v>
       </c>
       <c r="M7" t="n">
-        <v>14.7</v>
+        <v>7.7</v>
       </c>
       <c r="N7" t="n">
-        <v>14.3</v>
+        <v>7.3</v>
       </c>
       <c r="O7" t="n">
-        <v>13.9</v>
+        <v>6.9</v>
       </c>
       <c r="P7" t="n">
-        <v>13.5</v>
+        <v>6.5</v>
       </c>
       <c r="Q7" t="n">
-        <v>13.1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8">
@@ -1348,51 +1406,51 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>4.84</v>
+        <v>4.18</v>
       </c>
       <c r="D8" t="n">
-        <v>4.67</v>
+        <v>4.03</v>
       </c>
       <c r="E8" t="n">
-        <v>4.49</v>
+        <v>3.88</v>
       </c>
       <c r="F8" t="n">
-        <v>4.28</v>
+        <v>3.7</v>
       </c>
       <c r="G8" t="n">
-        <v>4.14</v>
+        <v>3.58</v>
       </c>
       <c r="H8" t="n">
-        <v>4.04</v>
+        <v>3.5</v>
       </c>
       <c r="I8" t="n">
-        <v>3.83</v>
+        <v>3.32</v>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>2.80 2.65 2.51 2.37</t>
+          <t>3.13 2.85 2.70 2.54</t>
         </is>
       </c>
       <c r="K8" t="n">
-        <v>2.27</v>
+        <v>2.43</v>
       </c>
       <c r="L8" t="n">
-        <v>2.21</v>
+        <v>2.37</v>
       </c>
       <c r="M8" t="n">
-        <v>2.04</v>
+        <v>2.18</v>
       </c>
       <c r="N8" t="n">
-        <v>1.86</v>
+        <v>1.98</v>
       </c>
       <c r="O8" t="n">
-        <v>1.67</v>
+        <v>1.77</v>
       </c>
       <c r="P8" t="n">
-        <v>1.46</v>
+        <v>1.55</v>
       </c>
       <c r="Q8" t="n">
-        <v>1.24</v>
+        <v>1.31</v>
       </c>
     </row>
     <row r="9">
@@ -1401,55 +1459,55 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>HI PR</t>
+          <t>EER</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>389</v>
+        <v>14.3</v>
       </c>
       <c r="D9" t="n">
-        <v>373</v>
+        <v>13.8</v>
       </c>
       <c r="E9" t="n">
-        <v>358</v>
+        <v>13.2</v>
       </c>
       <c r="F9" t="n">
-        <v>343</v>
+        <v>12.6</v>
       </c>
       <c r="G9" t="n">
-        <v>335</v>
+        <v>12.2</v>
       </c>
       <c r="H9" t="n">
-        <v>328</v>
+        <v>12</v>
       </c>
       <c r="I9" t="n">
-        <v>316</v>
+        <v>11.3</v>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>303 290 277 266</t>
+          <t>10.7 9.8 9.2 8.7</t>
         </is>
       </c>
       <c r="K9" t="n">
-        <v>260</v>
+        <v>8.300000000000001</v>
       </c>
       <c r="L9" t="n">
-        <v>255</v>
+        <v>8.1</v>
       </c>
       <c r="M9" t="n">
-        <v>245</v>
+        <v>7.4</v>
       </c>
       <c r="N9" t="n">
-        <v>236</v>
+        <v>6.8</v>
       </c>
       <c r="O9" t="n">
-        <v>226</v>
+        <v>6.1</v>
       </c>
       <c r="P9" t="n">
-        <v>218</v>
+        <v>5.3</v>
       </c>
       <c r="Q9" t="n">
-        <v>210</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="10">
@@ -1458,54 +1516,111 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
+          <t>HI PR</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>415</v>
+      </c>
+      <c r="D10" t="n">
+        <v>398</v>
+      </c>
+      <c r="E10" t="n">
+        <v>382</v>
+      </c>
+      <c r="F10" t="n">
+        <v>366</v>
+      </c>
+      <c r="G10" t="n">
+        <v>357</v>
+      </c>
+      <c r="H10" t="n">
+        <v>350</v>
+      </c>
+      <c r="I10" t="n">
+        <v>337</v>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>323 310 296 284</t>
+        </is>
+      </c>
+      <c r="K10" t="n">
+        <v>277</v>
+      </c>
+      <c r="L10" t="n">
+        <v>272</v>
+      </c>
+      <c r="M10" t="n">
+        <v>262</v>
+      </c>
+      <c r="N10" t="n">
+        <v>252</v>
+      </c>
+      <c r="O10" t="n">
+        <v>241</v>
+      </c>
+      <c r="P10" t="n">
+        <v>233</v>
+      </c>
+      <c r="Q10" t="n">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
           <t>LO PR</t>
         </is>
       </c>
-      <c r="C10" t="n">
-        <v>146</v>
-      </c>
-      <c r="D10" t="n">
-        <v>136</v>
-      </c>
-      <c r="E10" t="n">
-        <v>127</v>
-      </c>
-      <c r="F10" t="n">
-        <v>117</v>
-      </c>
-      <c r="G10" t="n">
-        <v>110</v>
-      </c>
-      <c r="H10" t="n">
-        <v>106</v>
-      </c>
-      <c r="I10" t="n">
-        <v>98</v>
-      </c>
-      <c r="J10" t="inlineStr">
-        <is>
-          <t>87 78 70 62</t>
-        </is>
-      </c>
-      <c r="K10" t="n">
-        <v>57</v>
-      </c>
-      <c r="L10" t="n">
-        <v>55</v>
-      </c>
-      <c r="M10" t="n">
-        <v>47</v>
-      </c>
-      <c r="N10" t="n">
-        <v>40</v>
-      </c>
-      <c r="O10" t="n">
-        <v>34</v>
-      </c>
-      <c r="P10" t="n">
-        <v>30</v>
-      </c>
-      <c r="Q10" t="n">
+      <c r="C11" t="n">
+        <v>142</v>
+      </c>
+      <c r="D11" t="n">
+        <v>132</v>
+      </c>
+      <c r="E11" t="n">
+        <v>124</v>
+      </c>
+      <c r="F11" t="n">
+        <v>113</v>
+      </c>
+      <c r="G11" t="n">
+        <v>107</v>
+      </c>
+      <c r="H11" t="n">
+        <v>103</v>
+      </c>
+      <c r="I11" t="n">
+        <v>95</v>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>84 76 68 60</t>
+        </is>
+      </c>
+      <c r="K11" t="n">
+        <v>56</v>
+      </c>
+      <c r="L11" t="n">
+        <v>54</v>
+      </c>
+      <c r="M11" t="n">
+        <v>45</v>
+      </c>
+      <c r="N11" t="n">
+        <v>39</v>
+      </c>
+      <c r="O11" t="n">
+        <v>33</v>
+      </c>
+      <c r="P11" t="n">
+        <v>29</v>
+      </c>
+      <c r="Q11" t="n">
         <v>23</v>
       </c>
     </row>
@@ -1520,7 +1635,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q10"/>
+  <dimension ref="A1:Q11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1666,51 +1781,51 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>58.3</v>
+        <v>43.4</v>
       </c>
       <c r="D4" t="n">
-        <v>54.6</v>
+        <v>41</v>
       </c>
       <c r="E4" t="n">
-        <v>50.9</v>
+        <v>38.6</v>
       </c>
       <c r="F4" t="n">
-        <v>47.3</v>
+        <v>36.1</v>
       </c>
       <c r="G4" t="n">
-        <v>45</v>
+        <v>34.5</v>
       </c>
       <c r="H4" t="n">
-        <v>43.3</v>
+        <v>33.4</v>
       </c>
       <c r="I4" t="n">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>45.5 42.4 39.1 36.0</t>
+          <t>28.6 24.6 22.7 20.9</t>
         </is>
       </c>
       <c r="K4" t="n">
-        <v>34</v>
+        <v>19.8</v>
       </c>
       <c r="L4" t="n">
-        <v>32.7</v>
+        <v>19</v>
       </c>
       <c r="M4" t="n">
-        <v>29.4</v>
+        <v>17.1</v>
       </c>
       <c r="N4" t="n">
-        <v>26</v>
+        <v>15.2</v>
       </c>
       <c r="O4" t="n">
-        <v>22.7</v>
+        <v>13.2</v>
       </c>
       <c r="P4" t="n">
-        <v>19.4</v>
+        <v>11.3</v>
       </c>
       <c r="Q4" t="n">
-        <v>15.9</v>
+        <v>9.199999999999999</v>
       </c>
     </row>
     <row r="5">
@@ -1723,51 +1838,51 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>36</v>
+        <v>33.5</v>
       </c>
       <c r="D5" t="n">
-        <v>34</v>
+        <v>31.7</v>
       </c>
       <c r="E5" t="n">
-        <v>32</v>
+        <v>29.8</v>
       </c>
       <c r="F5" t="n">
-        <v>30</v>
+        <v>27.9</v>
       </c>
       <c r="G5" t="n">
-        <v>29</v>
+        <v>26.6</v>
       </c>
       <c r="H5" t="n">
-        <v>28</v>
+        <v>25.8</v>
       </c>
       <c r="I5" t="n">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>29 27 25 23</t>
+          <t>22.1 19.0 17.6 16.2</t>
         </is>
       </c>
       <c r="K5" t="n">
-        <v>22</v>
+        <v>15.3</v>
       </c>
       <c r="L5" t="n">
-        <v>21</v>
+        <v>14.7</v>
       </c>
       <c r="M5" t="n">
-        <v>19</v>
+        <v>13.2</v>
       </c>
       <c r="N5" t="n">
-        <v>17</v>
+        <v>11.7</v>
       </c>
       <c r="O5" t="n">
-        <v>15</v>
+        <v>10.2</v>
       </c>
       <c r="P5" t="n">
-        <v>12</v>
+        <v>8.699999999999999</v>
       </c>
       <c r="Q5" t="n">
-        <v>10</v>
+        <v>7.1</v>
       </c>
     </row>
     <row r="6">
@@ -1780,51 +1895,51 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>3.8</v>
+        <v>3.2</v>
       </c>
       <c r="D6" t="n">
-        <v>3.73</v>
+        <v>3.14</v>
       </c>
       <c r="E6" t="n">
-        <v>3.66</v>
+        <v>3.07</v>
       </c>
       <c r="F6" t="n">
-        <v>3.59</v>
+        <v>3.01</v>
       </c>
       <c r="G6" t="n">
-        <v>3.55</v>
+        <v>2.97</v>
       </c>
       <c r="H6" t="n">
-        <v>3.52</v>
+        <v>2.94</v>
       </c>
       <c r="I6" t="n">
-        <v>3.45</v>
+        <v>2.88</v>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>4.57 4.46 4.34 4.22</t>
+          <t>2.82 2.49 2.43 2.37</t>
         </is>
       </c>
       <c r="K6" t="n">
-        <v>4.15</v>
+        <v>2.34</v>
       </c>
       <c r="L6" t="n">
-        <v>4.11</v>
+        <v>2.32</v>
       </c>
       <c r="M6" t="n">
-        <v>3.99</v>
+        <v>2.26</v>
       </c>
       <c r="N6" t="n">
-        <v>3.87</v>
+        <v>2.2</v>
       </c>
       <c r="O6" t="n">
-        <v>3.75</v>
+        <v>2.15</v>
       </c>
       <c r="P6" t="n">
-        <v>3.63</v>
+        <v>2.09</v>
       </c>
       <c r="Q6" t="n">
-        <v>3.52</v>
+        <v>2.04</v>
       </c>
     </row>
     <row r="7">
@@ -1837,51 +1952,51 @@
         </is>
       </c>
       <c r="C7" t="n">
+        <v>16.1</v>
+      </c>
+      <c r="D7" t="n">
+        <v>15.1</v>
+      </c>
+      <c r="E7" t="n">
         <v>14.2</v>
       </c>
-      <c r="D7" t="n">
-        <v>13.9</v>
-      </c>
-      <c r="E7" t="n">
-        <v>13.6</v>
-      </c>
       <c r="F7" t="n">
-        <v>13.3</v>
+        <v>13.4</v>
       </c>
       <c r="G7" t="n">
-        <v>13.1</v>
+        <v>13</v>
       </c>
       <c r="H7" t="n">
-        <v>13</v>
+        <v>12.8</v>
       </c>
       <c r="I7" t="n">
-        <v>12.7</v>
+        <v>12.1</v>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>18.7 18.2 17.7 17.2</t>
+          <t>11.6 11.1 10.7 10.3</t>
         </is>
       </c>
       <c r="K7" t="n">
-        <v>16.9</v>
+        <v>10.1</v>
       </c>
       <c r="L7" t="n">
-        <v>16.7</v>
+        <v>9.9</v>
       </c>
       <c r="M7" t="n">
-        <v>16.2</v>
+        <v>9.5</v>
       </c>
       <c r="N7" t="n">
-        <v>15.7</v>
+        <v>9</v>
       </c>
       <c r="O7" t="n">
-        <v>15.2</v>
+        <v>8.5</v>
       </c>
       <c r="P7" t="n">
-        <v>14.6</v>
+        <v>8</v>
       </c>
       <c r="Q7" t="n">
-        <v>14.1</v>
+        <v>7.3</v>
       </c>
     </row>
     <row r="8">
@@ -1894,51 +2009,51 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>4.49</v>
+        <v>3.96</v>
       </c>
       <c r="D8" t="n">
-        <v>4.29</v>
+        <v>3.83</v>
       </c>
       <c r="E8" t="n">
-        <v>4.08</v>
+        <v>3.68</v>
       </c>
       <c r="F8" t="n">
-        <v>3.86</v>
+        <v>3.52</v>
       </c>
       <c r="G8" t="n">
-        <v>3.72</v>
+        <v>3.4</v>
       </c>
       <c r="H8" t="n">
-        <v>3.61</v>
+        <v>3.32</v>
       </c>
       <c r="I8" t="n">
-        <v>3.32</v>
+        <v>3.15</v>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>2.91 2.79 2.64 2.50</t>
+          <t>2.98 2.90 2.74 2.58</t>
         </is>
       </c>
       <c r="K8" t="n">
-        <v>2.4</v>
+        <v>2.47</v>
       </c>
       <c r="L8" t="n">
-        <v>2.34</v>
+        <v>2.41</v>
       </c>
       <c r="M8" t="n">
-        <v>2.16</v>
+        <v>2.21</v>
       </c>
       <c r="N8" t="n">
-        <v>1.97</v>
+        <v>2.01</v>
       </c>
       <c r="O8" t="n">
-        <v>1.77</v>
+        <v>1.8</v>
       </c>
       <c r="P8" t="n">
-        <v>1.56</v>
+        <v>1.58</v>
       </c>
       <c r="Q8" t="n">
-        <v>1.32</v>
+        <v>1.33</v>
       </c>
     </row>
     <row r="9">
@@ -1947,55 +2062,55 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>HI PR</t>
+          <t>EER</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>378</v>
+        <v>13.5</v>
       </c>
       <c r="D9" t="n">
-        <v>366</v>
+        <v>13.1</v>
       </c>
       <c r="E9" t="n">
-        <v>354</v>
+        <v>12.6</v>
       </c>
       <c r="F9" t="n">
-        <v>341</v>
+        <v>12</v>
       </c>
       <c r="G9" t="n">
-        <v>334</v>
+        <v>11.6</v>
       </c>
       <c r="H9" t="n">
-        <v>329</v>
+        <v>11.4</v>
       </c>
       <c r="I9" t="n">
-        <v>317</v>
+        <v>10.8</v>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>302 289 276 265</t>
+          <t>10.2 9.9 9.4 8.8</t>
         </is>
       </c>
       <c r="K9" t="n">
-        <v>259</v>
+        <v>8.5</v>
       </c>
       <c r="L9" t="n">
-        <v>254</v>
+        <v>8.199999999999999</v>
       </c>
       <c r="M9" t="n">
-        <v>245</v>
+        <v>7.6</v>
       </c>
       <c r="N9" t="n">
-        <v>235</v>
+        <v>6.9</v>
       </c>
       <c r="O9" t="n">
-        <v>226</v>
+        <v>6.1</v>
       </c>
       <c r="P9" t="n">
-        <v>218</v>
+        <v>5.4</v>
       </c>
       <c r="Q9" t="n">
-        <v>210</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="10">
@@ -2004,55 +2119,112 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
+          <t>HI PR</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>464</v>
+      </c>
+      <c r="D10" t="n">
+        <v>445</v>
+      </c>
+      <c r="E10" t="n">
+        <v>428</v>
+      </c>
+      <c r="F10" t="n">
+        <v>409</v>
+      </c>
+      <c r="G10" t="n">
+        <v>399</v>
+      </c>
+      <c r="H10" t="n">
+        <v>392</v>
+      </c>
+      <c r="I10" t="n">
+        <v>376</v>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>361 346 331 317</t>
+        </is>
+      </c>
+      <c r="K10" t="n">
+        <v>310</v>
+      </c>
+      <c r="L10" t="n">
+        <v>304</v>
+      </c>
+      <c r="M10" t="n">
+        <v>293</v>
+      </c>
+      <c r="N10" t="n">
+        <v>281</v>
+      </c>
+      <c r="O10" t="n">
+        <v>270</v>
+      </c>
+      <c r="P10" t="n">
+        <v>260</v>
+      </c>
+      <c r="Q10" t="n">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
           <t>LO PR</t>
         </is>
       </c>
-      <c r="C10" t="n">
+      <c r="C11" t="n">
         <v>139</v>
       </c>
-      <c r="D10" t="n">
-        <v>131</v>
-      </c>
-      <c r="E10" t="n">
-        <v>122</v>
-      </c>
-      <c r="F10" t="n">
-        <v>113</v>
-      </c>
-      <c r="G10" t="n">
-        <v>108</v>
-      </c>
-      <c r="H10" t="n">
+      <c r="D11" t="n">
+        <v>129</v>
+      </c>
+      <c r="E11" t="n">
+        <v>121</v>
+      </c>
+      <c r="F11" t="n">
+        <v>111</v>
+      </c>
+      <c r="G11" t="n">
         <v>105</v>
       </c>
-      <c r="I10" t="n">
-        <v>96</v>
-      </c>
-      <c r="J10" t="inlineStr">
-        <is>
-          <t>85 77 69 60</t>
-        </is>
-      </c>
-      <c r="K10" t="n">
-        <v>56</v>
-      </c>
-      <c r="L10" t="n">
+      <c r="H11" t="n">
+        <v>101</v>
+      </c>
+      <c r="I11" t="n">
+        <v>92</v>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>82 74 66 58</t>
+        </is>
+      </c>
+      <c r="K11" t="n">
         <v>54</v>
       </c>
-      <c r="M10" t="n">
-        <v>46</v>
-      </c>
-      <c r="N10" t="n">
-        <v>39</v>
-      </c>
-      <c r="O10" t="n">
-        <v>33</v>
-      </c>
-      <c r="P10" t="n">
-        <v>29</v>
-      </c>
-      <c r="Q10" t="n">
-        <v>23</v>
+      <c r="L11" t="n">
+        <v>52</v>
+      </c>
+      <c r="M11" t="n">
+        <v>44</v>
+      </c>
+      <c r="N11" t="n">
+        <v>38</v>
+      </c>
+      <c r="O11" t="n">
+        <v>32</v>
+      </c>
+      <c r="P11" t="n">
+        <v>28</v>
+      </c>
+      <c r="Q11" t="n">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -2066,7 +2238,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q10"/>
+  <dimension ref="A1:Q11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2212,51 +2384,51 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>63.2</v>
+        <v>52.9</v>
       </c>
       <c r="D4" t="n">
-        <v>59.5</v>
+        <v>50</v>
       </c>
       <c r="E4" t="n">
-        <v>55.9</v>
+        <v>47.1</v>
       </c>
       <c r="F4" t="n">
-        <v>52.3</v>
+        <v>44</v>
       </c>
       <c r="G4" t="n">
-        <v>50</v>
+        <v>42.1</v>
       </c>
       <c r="H4" t="n">
-        <v>48.3</v>
+        <v>40.7</v>
       </c>
       <c r="I4" t="n">
-        <v>44.2</v>
+        <v>37.8</v>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>47.6 43.6 40.6 38.5</t>
+          <t>34.9 30.1 27.8 25.6</t>
         </is>
       </c>
       <c r="K4" t="n">
-        <v>37.3</v>
+        <v>24.2</v>
       </c>
       <c r="L4" t="n">
-        <v>35.8</v>
+        <v>23.3</v>
       </c>
       <c r="M4" t="n">
-        <v>32.1</v>
+        <v>20.9</v>
       </c>
       <c r="N4" t="n">
-        <v>28.3</v>
+        <v>18.5</v>
       </c>
       <c r="O4" t="n">
-        <v>24.6</v>
+        <v>16.1</v>
       </c>
       <c r="P4" t="n">
-        <v>20.8</v>
+        <v>13.8</v>
       </c>
       <c r="Q4" t="n">
-        <v>17.1</v>
+        <v>11.3</v>
       </c>
     </row>
     <row r="5">
@@ -2272,48 +2444,48 @@
         <v>35</v>
       </c>
       <c r="D5" t="n">
-        <v>33</v>
+        <v>33.1</v>
       </c>
       <c r="E5" t="n">
-        <v>31</v>
+        <v>31.1</v>
       </c>
       <c r="F5" t="n">
-        <v>29</v>
+        <v>29.1</v>
       </c>
       <c r="G5" t="n">
-        <v>28</v>
+        <v>27.8</v>
       </c>
       <c r="H5" t="n">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I5" t="n">
         <v>25</v>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>27 25 23 22</t>
+          <t>23.1 19.9 18.4 16.9</t>
         </is>
       </c>
       <c r="K5" t="n">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="L5" t="n">
-        <v>20</v>
+        <v>15.4</v>
       </c>
       <c r="M5" t="n">
-        <v>18</v>
+        <v>13.8</v>
       </c>
       <c r="N5" t="n">
-        <v>16</v>
+        <v>12.2</v>
       </c>
       <c r="O5" t="n">
-        <v>14</v>
+        <v>10.7</v>
       </c>
       <c r="P5" t="n">
-        <v>12</v>
+        <v>9.1</v>
       </c>
       <c r="Q5" t="n">
-        <v>10</v>
+        <v>7.5</v>
       </c>
     </row>
     <row r="6">
@@ -2326,51 +2498,51 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>4.29</v>
+        <v>3.58</v>
       </c>
       <c r="D6" t="n">
-        <v>4.2</v>
+        <v>3.51</v>
       </c>
       <c r="E6" t="n">
-        <v>4.12</v>
+        <v>3.44</v>
       </c>
       <c r="F6" t="n">
-        <v>4.03</v>
+        <v>3.37</v>
       </c>
       <c r="G6" t="n">
-        <v>3.98</v>
+        <v>3.33</v>
       </c>
       <c r="H6" t="n">
-        <v>3.95</v>
+        <v>3.3</v>
       </c>
       <c r="I6" t="n">
-        <v>3.86</v>
+        <v>3.23</v>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>4.96 4.83 4.69 4.56</t>
+          <t>3.16 3.01 2.95 2.88</t>
         </is>
       </c>
       <c r="K6" t="n">
-        <v>4.48</v>
+        <v>2.84</v>
       </c>
       <c r="L6" t="n">
-        <v>4.42</v>
+        <v>2.82</v>
       </c>
       <c r="M6" t="n">
-        <v>4.29</v>
+        <v>2.75</v>
       </c>
       <c r="N6" t="n">
-        <v>4.15</v>
+        <v>2.68</v>
       </c>
       <c r="O6" t="n">
-        <v>4.02</v>
+        <v>2.62</v>
       </c>
       <c r="P6" t="n">
-        <v>3.89</v>
+        <v>2.55</v>
       </c>
       <c r="Q6" t="n">
-        <v>3.75</v>
+        <v>2.49</v>
       </c>
     </row>
     <row r="7">
@@ -2383,51 +2555,51 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>16.1</v>
+        <v>18.1</v>
       </c>
       <c r="D7" t="n">
-        <v>15.7</v>
+        <v>16.8</v>
       </c>
       <c r="E7" t="n">
-        <v>15.3</v>
+        <v>15.9</v>
       </c>
       <c r="F7" t="n">
-        <v>14.9</v>
+        <v>15</v>
       </c>
       <c r="G7" t="n">
-        <v>14.7</v>
+        <v>14.5</v>
       </c>
       <c r="H7" t="n">
-        <v>14.6</v>
+        <v>14.3</v>
       </c>
       <c r="I7" t="n">
-        <v>14.2</v>
+        <v>13.5</v>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>19.0 18.4 17.8 17.2</t>
+          <t>12.9 12.4 12.0 11.5</t>
         </is>
       </c>
       <c r="K7" t="n">
-        <v>16.9</v>
+        <v>11.2</v>
       </c>
       <c r="L7" t="n">
-        <v>16.6</v>
+        <v>11.1</v>
       </c>
       <c r="M7" t="n">
-        <v>16</v>
+        <v>10.6</v>
       </c>
       <c r="N7" t="n">
-        <v>15.5</v>
+        <v>10</v>
       </c>
       <c r="O7" t="n">
-        <v>14.9</v>
+        <v>9.5</v>
       </c>
       <c r="P7" t="n">
-        <v>14.3</v>
+        <v>8.9</v>
       </c>
       <c r="Q7" t="n">
-        <v>13.7</v>
+        <v>8.199999999999999</v>
       </c>
     </row>
     <row r="8">
@@ -2440,48 +2612,48 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>4.32</v>
+        <v>4.33</v>
       </c>
       <c r="D8" t="n">
-        <v>4.15</v>
+        <v>4.18</v>
       </c>
       <c r="E8" t="n">
-        <v>3.98</v>
+        <v>4.01</v>
       </c>
       <c r="F8" t="n">
-        <v>3.8</v>
+        <v>3.82</v>
       </c>
       <c r="G8" t="n">
-        <v>3.68</v>
+        <v>3.7</v>
       </c>
       <c r="H8" t="n">
-        <v>3.59</v>
+        <v>3.61</v>
       </c>
       <c r="I8" t="n">
-        <v>3.35</v>
+        <v>3.43</v>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>2.81 2.65 2.54 2.47</t>
+          <t>3.23 2.92 2.76 2.60</t>
         </is>
       </c>
       <c r="K8" t="n">
-        <v>2.44</v>
+        <v>2.49</v>
       </c>
       <c r="L8" t="n">
-        <v>2.37</v>
+        <v>2.42</v>
       </c>
       <c r="M8" t="n">
-        <v>2.19</v>
+        <v>2.22</v>
       </c>
       <c r="N8" t="n">
-        <v>2</v>
+        <v>2.02</v>
       </c>
       <c r="O8" t="n">
-        <v>1.79</v>
+        <v>1.8</v>
       </c>
       <c r="P8" t="n">
-        <v>1.57</v>
+        <v>1.58</v>
       </c>
       <c r="Q8" t="n">
         <v>1.33</v>
@@ -2493,55 +2665,55 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>HI PR</t>
+          <t>EER</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>381</v>
+        <v>14.8</v>
       </c>
       <c r="D9" t="n">
-        <v>369</v>
+        <v>14.3</v>
       </c>
       <c r="E9" t="n">
-        <v>356</v>
+        <v>13.7</v>
       </c>
       <c r="F9" t="n">
-        <v>344</v>
+        <v>13.1</v>
       </c>
       <c r="G9" t="n">
-        <v>337</v>
+        <v>12.6</v>
       </c>
       <c r="H9" t="n">
-        <v>332</v>
+        <v>12.3</v>
       </c>
       <c r="I9" t="n">
-        <v>319</v>
+        <v>11.7</v>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>331 318 305 291</t>
+          <t>11.0 10.0 9.4 8.9</t>
         </is>
       </c>
       <c r="K9" t="n">
-        <v>283</v>
+        <v>8.5</v>
       </c>
       <c r="L9" t="n">
-        <v>278</v>
+        <v>8.300000000000001</v>
       </c>
       <c r="M9" t="n">
-        <v>264</v>
+        <v>7.6</v>
       </c>
       <c r="N9" t="n">
-        <v>251</v>
+        <v>6.9</v>
       </c>
       <c r="O9" t="n">
-        <v>238</v>
+        <v>6.2</v>
       </c>
       <c r="P9" t="n">
-        <v>224</v>
+        <v>5.4</v>
       </c>
       <c r="Q9" t="n">
-        <v>211</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="10">
@@ -2550,55 +2722,715 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
+          <t>HI PR</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>414</v>
+      </c>
+      <c r="D10" t="n">
+        <v>397</v>
+      </c>
+      <c r="E10" t="n">
+        <v>382</v>
+      </c>
+      <c r="F10" t="n">
+        <v>365</v>
+      </c>
+      <c r="G10" t="n">
+        <v>357</v>
+      </c>
+      <c r="H10" t="n">
+        <v>350</v>
+      </c>
+      <c r="I10" t="n">
+        <v>336</v>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>323 309 295 283</t>
+        </is>
+      </c>
+      <c r="K10" t="n">
+        <v>277</v>
+      </c>
+      <c r="L10" t="n">
+        <v>272</v>
+      </c>
+      <c r="M10" t="n">
+        <v>261</v>
+      </c>
+      <c r="N10" t="n">
+        <v>251</v>
+      </c>
+      <c r="O10" t="n">
+        <v>241</v>
+      </c>
+      <c r="P10" t="n">
+        <v>232</v>
+      </c>
+      <c r="Q10" t="n">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
           <t>LO PR</t>
         </is>
       </c>
+      <c r="C11" t="n">
+        <v>142</v>
+      </c>
+      <c r="D11" t="n">
+        <v>132</v>
+      </c>
+      <c r="E11" t="n">
+        <v>123</v>
+      </c>
+      <c r="F11" t="n">
+        <v>113</v>
+      </c>
+      <c r="G11" t="n">
+        <v>107</v>
+      </c>
+      <c r="H11" t="n">
+        <v>103</v>
+      </c>
+      <c r="I11" t="n">
+        <v>95</v>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>84 76 68 60</t>
+        </is>
+      </c>
+      <c r="K11" t="n">
+        <v>55</v>
+      </c>
+      <c r="L11" t="n">
+        <v>53</v>
+      </c>
+      <c r="M11" t="n">
+        <v>45</v>
+      </c>
+      <c r="N11" t="n">
+        <v>39</v>
+      </c>
+      <c r="O11" t="n">
+        <v>33</v>
+      </c>
+      <c r="P11" t="n">
+        <v>29</v>
+      </c>
+      <c r="Q11" t="n">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:Q11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="J1" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="K1" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="L1" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="M1" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="N1" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="O1" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="P1" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="Q1" s="1" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="inlineStr"/>
+      <c r="C2" t="inlineStr"/>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="inlineStr"/>
+      <c r="H2" t="inlineStr"/>
+      <c r="I2" t="inlineStr"/>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>Outdoor Ambient Temperature</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr"/>
+      <c r="L2" t="inlineStr"/>
+      <c r="M2" t="inlineStr"/>
+      <c r="N2" t="inlineStr"/>
+      <c r="O2" t="inlineStr"/>
+      <c r="P2" t="inlineStr"/>
+      <c r="Q2" t="inlineStr"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="inlineStr"/>
+      <c r="C3" t="n">
+        <v>65</v>
+      </c>
+      <c r="D3" t="n">
+        <v>60</v>
+      </c>
+      <c r="E3" t="n">
+        <v>55</v>
+      </c>
+      <c r="F3" t="n">
+        <v>50</v>
+      </c>
+      <c r="G3" t="n">
+        <v>47</v>
+      </c>
+      <c r="H3" t="n">
+        <v>45</v>
+      </c>
+      <c r="I3" t="n">
+        <v>40</v>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>35 30 25 20</t>
+        </is>
+      </c>
+      <c r="K3" t="n">
+        <v>17</v>
+      </c>
+      <c r="L3" t="n">
+        <v>15</v>
+      </c>
+      <c r="M3" t="n">
+        <v>10</v>
+      </c>
+      <c r="N3" t="n">
+        <v>5</v>
+      </c>
+      <c r="O3" t="n">
+        <v>0</v>
+      </c>
+      <c r="P3" t="n">
+        <v>-5</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>MBh</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>56.7</v>
+      </c>
+      <c r="D4" t="n">
+        <v>53.7</v>
+      </c>
+      <c r="E4" t="n">
+        <v>50.5</v>
+      </c>
+      <c r="F4" t="n">
+        <v>47.2</v>
+      </c>
+      <c r="G4" t="n">
+        <v>45.1</v>
+      </c>
+      <c r="H4" t="n">
+        <v>43.7</v>
+      </c>
+      <c r="I4" t="n">
+        <v>40.6</v>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>37.4 32.8 30.3 27.9</t>
+        </is>
+      </c>
+      <c r="K4" t="n">
+        <v>26.3</v>
+      </c>
+      <c r="L4" t="n">
+        <v>25.3</v>
+      </c>
+      <c r="M4" t="n">
+        <v>22.7</v>
+      </c>
+      <c r="N4" t="n">
+        <v>20.2</v>
+      </c>
+      <c r="O4" t="n">
+        <v>17.6</v>
+      </c>
+      <c r="P4" t="n">
+        <v>15</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>12.3</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>T/R</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>33.9</v>
+      </c>
+      <c r="D5" t="n">
+        <v>32.1</v>
+      </c>
+      <c r="E5" t="n">
+        <v>30.2</v>
+      </c>
+      <c r="F5" t="n">
+        <v>28.2</v>
+      </c>
+      <c r="G5" t="n">
+        <v>26.9</v>
+      </c>
+      <c r="H5" t="n">
+        <v>26.1</v>
+      </c>
+      <c r="I5" t="n">
+        <v>24.2</v>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>22.4 19.6 18.1 16.6</t>
+        </is>
+      </c>
+      <c r="K5" t="n">
+        <v>15.7</v>
+      </c>
+      <c r="L5" t="n">
+        <v>15.1</v>
+      </c>
+      <c r="M5" t="n">
+        <v>13.6</v>
+      </c>
+      <c r="N5" t="n">
+        <v>12</v>
+      </c>
+      <c r="O5" t="n">
+        <v>10.5</v>
+      </c>
+      <c r="P5" t="n">
+        <v>9</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>7.3</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>kW</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>3.92</v>
+      </c>
+      <c r="D6" t="n">
+        <v>3.85</v>
+      </c>
+      <c r="E6" t="n">
+        <v>3.77</v>
+      </c>
+      <c r="F6" t="n">
+        <v>3.7</v>
+      </c>
+      <c r="G6" t="n">
+        <v>3.65</v>
+      </c>
+      <c r="H6" t="n">
+        <v>3.62</v>
+      </c>
+      <c r="I6" t="n">
+        <v>3.55</v>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>3.48 3.31 3.24 3.17</t>
+        </is>
+      </c>
+      <c r="K6" t="n">
+        <v>3.12</v>
+      </c>
+      <c r="L6" t="n">
+        <v>3.1</v>
+      </c>
+      <c r="M6" t="n">
+        <v>3.02</v>
+      </c>
+      <c r="N6" t="n">
+        <v>2.95</v>
+      </c>
+      <c r="O6" t="n">
+        <v>2.88</v>
+      </c>
+      <c r="P6" t="n">
+        <v>2.81</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>2.74</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Amps</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>19.4</v>
+      </c>
+      <c r="D7" t="n">
+        <v>18.1</v>
+      </c>
+      <c r="E7" t="n">
+        <v>17.1</v>
+      </c>
+      <c r="F7" t="n">
+        <v>16.2</v>
+      </c>
+      <c r="G7" t="n">
+        <v>15.7</v>
+      </c>
+      <c r="H7" t="n">
+        <v>15.4</v>
+      </c>
+      <c r="I7" t="n">
+        <v>14.6</v>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>14.0 13.5 12.9 12.4</t>
+        </is>
+      </c>
+      <c r="K7" t="n">
+        <v>12.2</v>
+      </c>
+      <c r="L7" t="n">
+        <v>12</v>
+      </c>
+      <c r="M7" t="n">
+        <v>11.5</v>
+      </c>
+      <c r="N7" t="n">
+        <v>10.9</v>
+      </c>
+      <c r="O7" t="n">
+        <v>10.3</v>
+      </c>
+      <c r="P7" t="n">
+        <v>9.699999999999999</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>8.9</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>COP</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>4.23</v>
+      </c>
+      <c r="D8" t="n">
+        <v>4.08</v>
+      </c>
+      <c r="E8" t="n">
+        <v>3.92</v>
+      </c>
+      <c r="F8" t="n">
+        <v>3.74</v>
+      </c>
+      <c r="G8" t="n">
+        <v>3.61</v>
+      </c>
+      <c r="H8" t="n">
+        <v>3.53</v>
+      </c>
+      <c r="I8" t="n">
+        <v>3.35</v>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>3.15 2.90 2.74 2.58</t>
+        </is>
+      </c>
+      <c r="K8" t="n">
+        <v>2.46</v>
+      </c>
+      <c r="L8" t="n">
+        <v>2.39</v>
+      </c>
+      <c r="M8" t="n">
+        <v>2.2</v>
+      </c>
+      <c r="N8" t="n">
+        <v>2</v>
+      </c>
+      <c r="O8" t="n">
+        <v>1.78</v>
+      </c>
+      <c r="P8" t="n">
+        <v>1.56</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>1.31</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>EER</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>14.5</v>
+      </c>
+      <c r="D9" t="n">
+        <v>14</v>
+      </c>
+      <c r="E9" t="n">
+        <v>13.4</v>
+      </c>
+      <c r="F9" t="n">
+        <v>12.8</v>
+      </c>
+      <c r="G9" t="n">
+        <v>12.3</v>
+      </c>
+      <c r="H9" t="n">
+        <v>12.1</v>
+      </c>
+      <c r="I9" t="n">
+        <v>11.4</v>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>10.8 9.9 9.3 8.8</t>
+        </is>
+      </c>
+      <c r="K9" t="n">
+        <v>8.4</v>
+      </c>
+      <c r="L9" t="n">
+        <v>8.199999999999999</v>
+      </c>
+      <c r="M9" t="n">
+        <v>7.5</v>
+      </c>
+      <c r="N9" t="n">
+        <v>6.8</v>
+      </c>
+      <c r="O9" t="n">
+        <v>6.1</v>
+      </c>
+      <c r="P9" t="n">
+        <v>5.3</v>
+      </c>
+      <c r="Q9" t="n">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>HI PR</t>
+        </is>
+      </c>
       <c r="C10" t="n">
-        <v>140</v>
+        <v>406</v>
       </c>
       <c r="D10" t="n">
-        <v>131</v>
+        <v>389</v>
       </c>
       <c r="E10" t="n">
+        <v>374</v>
+      </c>
+      <c r="F10" t="n">
+        <v>358</v>
+      </c>
+      <c r="G10" t="n">
+        <v>349</v>
+      </c>
+      <c r="H10" t="n">
+        <v>343</v>
+      </c>
+      <c r="I10" t="n">
+        <v>329</v>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>316 303 289 278</t>
+        </is>
+      </c>
+      <c r="K10" t="n">
+        <v>271</v>
+      </c>
+      <c r="L10" t="n">
+        <v>266</v>
+      </c>
+      <c r="M10" t="n">
+        <v>256</v>
+      </c>
+      <c r="N10" t="n">
+        <v>246</v>
+      </c>
+      <c r="O10" t="n">
+        <v>236</v>
+      </c>
+      <c r="P10" t="n">
+        <v>228</v>
+      </c>
+      <c r="Q10" t="n">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>LO PR</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>132</v>
+      </c>
+      <c r="D11" t="n">
         <v>122</v>
       </c>
-      <c r="F10" t="n">
-        <v>114</v>
-      </c>
-      <c r="G10" t="n">
-        <v>109</v>
-      </c>
-      <c r="H10" t="n">
+      <c r="E11" t="n">
+        <v>115</v>
+      </c>
+      <c r="F11" t="n">
         <v>105</v>
       </c>
-      <c r="I10" t="n">
+      <c r="G11" t="n">
+        <v>99</v>
+      </c>
+      <c r="H11" t="n">
         <v>96</v>
       </c>
-      <c r="J10" t="inlineStr">
-        <is>
-          <t>86 77 69 60</t>
-        </is>
-      </c>
-      <c r="K10" t="n">
-        <v>55</v>
-      </c>
-      <c r="L10" t="n">
+      <c r="I11" t="n">
+        <v>88</v>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>78 71 63 55</t>
+        </is>
+      </c>
+      <c r="K11" t="n">
         <v>52</v>
       </c>
-      <c r="M10" t="n">
-        <v>43</v>
-      </c>
-      <c r="N10" t="n">
-        <v>35</v>
-      </c>
-      <c r="O10" t="n">
-        <v>26</v>
-      </c>
-      <c r="P10" t="n">
-        <v>18</v>
-      </c>
-      <c r="Q10" t="n">
-        <v>9</v>
+      <c r="L11" t="n">
+        <v>50</v>
+      </c>
+      <c r="M11" t="n">
+        <v>42</v>
+      </c>
+      <c r="N11" t="n">
+        <v>36</v>
+      </c>
+      <c r="O11" t="n">
+        <v>31</v>
+      </c>
+      <c r="P11" t="n">
+        <v>27</v>
+      </c>
+      <c r="Q11" t="n">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>